<commit_message>
Added test cases TC156
</commit_message>
<xml_diff>
--- a/test-data/data.xlsx
+++ b/test-data/data.xlsx
@@ -7,12 +7,29 @@
     <workbookView xWindow="0" yWindow="108" windowWidth="15300" windowHeight="7968"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="TC156" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>manager</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -34,7 +51,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +59,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -349,12 +382,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="240" zoomScaleNormal="240" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>